<commit_message>
Did Changes in Linear Process
</commit_message>
<xml_diff>
--- a/Linear Process Workflow/Create case.xlsx
+++ b/Linear Process Workflow/Create case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anjani\Documents\UiPath\NABARD_Create case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anjani\Documents\UiPath\Nabard_Linear Process\Linear Process Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2D890-8F04-4C09-963C-26BD8C5EB179}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2EDE2C-A895-4B8A-8CC9-E524EBC9B5E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E8CC490B-AC56-4F82-B3D6-A1BC71FE64D9}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>rn.menon</t>
   </si>
   <si>
-    <t>NB-DFIBT-ADMN-CVC-2020-21-E-000100</t>
+    <t>NB-DFIBT-ADMN-CVC-2020-21-E-000103</t>
   </si>
 </sst>
 </file>

</xml_diff>